<commit_message>
Tweaking some missing values (eg. 'no' for measuring pain) Describing pain Fleshing out appendix Testing more moderators in models Cleaning up printing of quality graphs
</commit_message>
<xml_diff>
--- a/quality_review.xlsx
+++ b/quality_review.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2509920f_student_gla_ac_uk/Documents/DClin/Deliverables/Systematic Review/Writeup/DCLIN_SR_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="402" documentId="8_{BDA90F51-975A-4A3A-9E3C-A0EF38026AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73A2301A-7455-466C-A670-BFA1232BBDEC}"/>
+  <xr:revisionPtr revIDLastSave="404" documentId="8_{BDA90F51-975A-4A3A-9E3C-A0EF38026AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{11184E37-437E-4CB3-9E67-9303757942F1}"/>
   <bookViews>
-    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{960BDED2-1FF1-4B58-9DE1-81C8DE898166}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{960BDED2-1FF1-4B58-9DE1-81C8DE898166}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -436,9 +436,6 @@
     <t>LI_120</t>
   </si>
   <si>
-    <t>self-rated pain for both groups using IASP definition - 3 months or more. But no exclusions? Which is maybe acceptable for the nature of study (will get penalised later for confounds uncontrolled)</t>
-  </si>
-  <si>
     <t xml:space="preserve">Cluster sampling from rural elderly population and selection of 3 urban health centres. </t>
   </si>
   <si>
@@ -908,6 +905,9 @@
   </si>
   <si>
     <t>medication not controlled for. Depression and anxiety controlled for by exclusions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self-rated pain for both groups using IASP definition - 3 months or more. But no exclusions? </t>
   </si>
 </sst>
 </file>
@@ -1348,10 +1348,10 @@
   <dimension ref="A1:W55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="S51" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U55" sqref="U55"/>
+      <selection pane="bottomRight" activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.4"/>
@@ -1383,7 +1383,7 @@
   <sheetData>
     <row r="1" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>0</v>
@@ -1410,19 +1410,19 @@
         <v>7</v>
       </c>
       <c r="J1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="K1" s="6" t="s">
+        <v>254</v>
+      </c>
+      <c r="L1" s="6" t="s">
+        <v>262</v>
+      </c>
+      <c r="M1" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="K1" s="6" t="s">
-        <v>255</v>
-      </c>
-      <c r="L1" s="6" t="s">
-        <v>263</v>
-      </c>
-      <c r="M1" s="6" t="s">
+      <c r="N1" s="6" t="s">
         <v>252</v>
-      </c>
-      <c r="N1" s="6" t="s">
-        <v>253</v>
       </c>
       <c r="O1" s="6" t="s">
         <v>8</v>
@@ -1434,10 +1434,10 @@
         <v>10</v>
       </c>
       <c r="R1" s="6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="S1" s="6" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="T1" s="6" t="s">
         <v>11</v>
@@ -1479,7 +1479,7 @@
       </c>
       <c r="I2" s="8"/>
       <c r="J2" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K2" s="9" t="s">
         <v>21</v>
@@ -1499,10 +1499,10 @@
         <v>20</v>
       </c>
       <c r="R2" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S2" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T2" s="12" t="s">
         <v>21</v>
@@ -1544,7 +1544,7 @@
       </c>
       <c r="I3" s="8"/>
       <c r="J3" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K3" s="9" t="s">
         <v>21</v>
@@ -1564,16 +1564,16 @@
         <v>20</v>
       </c>
       <c r="R3" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S3" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T3" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U3" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V3" s="12" t="s">
         <v>16</v>
@@ -1605,7 +1605,7 @@
       <c r="H4" s="6"/>
       <c r="I4" s="8"/>
       <c r="J4" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K4" s="9" t="s">
         <v>21</v>
@@ -1625,16 +1625,16 @@
         <v>20</v>
       </c>
       <c r="R4" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S4" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T4" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U4" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V4" s="12" t="s">
         <v>21</v>
@@ -1680,7 +1680,7 @@
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O5" s="6" t="s">
         <v>36</v>
@@ -1695,13 +1695,13 @@
         <v>21</v>
       </c>
       <c r="S5" s="6" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="T5" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U5" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V5" s="12" t="s">
         <v>16</v>
@@ -1731,16 +1731,16 @@
         <v>34</v>
       </c>
       <c r="H6" s="6" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="I6" s="8" t="s">
         <v>34</v>
       </c>
       <c r="J6" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="K6" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L6" s="10" t="s">
         <v>21</v>
@@ -1750,7 +1750,7 @@
         <v>16</v>
       </c>
       <c r="O6" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="P6" s="8" t="s">
         <v>21</v>
@@ -1759,16 +1759,16 @@
         <v>42</v>
       </c>
       <c r="R6" s="6" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="S6" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T6" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U6" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V6" s="12" t="s">
         <v>16</v>
@@ -1800,10 +1800,10 @@
       <c r="H7" s="6"/>
       <c r="I7" s="8"/>
       <c r="J7" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K7" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L7" s="10" t="s">
         <v>21</v>
@@ -1822,10 +1822,10 @@
         <v>46</v>
       </c>
       <c r="R7" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S7" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T7" s="12" t="s">
         <v>34</v>
@@ -1863,13 +1863,13 @@
       <c r="H8" s="6"/>
       <c r="I8" s="8"/>
       <c r="J8" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K8" s="14" t="s">
         <v>21</v>
       </c>
       <c r="L8" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="6" t="s">
@@ -1885,10 +1885,10 @@
         <v>51</v>
       </c>
       <c r="R8" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S8" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T8" s="12" t="s">
         <v>34</v>
@@ -1955,7 +1955,7 @@
         <v>21</v>
       </c>
       <c r="S9" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T9" s="12" t="s">
         <v>16</v>
@@ -2000,7 +2000,7 @@
         <v>16</v>
       </c>
       <c r="K10" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L10" s="16" t="s">
         <v>21</v>
@@ -2022,13 +2022,13 @@
         <v>21</v>
       </c>
       <c r="S10" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T10" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U10" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V10" s="12" t="s">
         <v>16</v>
@@ -2046,7 +2046,7 @@
         <v>21</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>34</v>
@@ -2062,7 +2062,7 @@
       </c>
       <c r="I11" s="8"/>
       <c r="J11" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K11" s="14" t="s">
         <v>21</v>
@@ -2082,16 +2082,16 @@
         <v>20</v>
       </c>
       <c r="R11" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S11" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T11" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U11" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V11" s="12" t="s">
         <v>16</v>
@@ -2135,7 +2135,7 @@
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O12" s="6" t="s">
         <v>71</v>
@@ -2145,16 +2145,16 @@
         <v>20</v>
       </c>
       <c r="R12" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S12" s="6" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="T12" s="12" t="s">
         <v>34</v>
       </c>
       <c r="U12" s="12" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="V12" s="6" t="s">
         <v>34</v>
@@ -2180,7 +2180,7 @@
         <v>21</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="G13" s="8" t="s">
         <v>21</v>
@@ -2195,7 +2195,7 @@
         <v>16</v>
       </c>
       <c r="K13" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L13" s="16" t="s">
         <v>21</v>
@@ -2215,7 +2215,7 @@
         <v>21</v>
       </c>
       <c r="S13" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T13" s="12" t="s">
         <v>21</v>
@@ -2267,7 +2267,7 @@
       </c>
       <c r="M14" s="13"/>
       <c r="N14" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O14" s="6" t="s">
         <v>80</v>
@@ -2275,10 +2275,10 @@
       <c r="P14" s="8"/>
       <c r="Q14" s="6"/>
       <c r="R14" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="S14" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="S14" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="T14" s="12" t="s">
         <v>16</v>
@@ -2330,7 +2330,7 @@
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O15" s="6" t="s">
         <v>85</v>
@@ -2345,13 +2345,13 @@
         <v>21</v>
       </c>
       <c r="S15" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T15" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U15" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V15" s="12" t="s">
         <v>16</v>
@@ -2363,13 +2363,13 @@
         <v>87</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C16" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>16</v>
@@ -2388,7 +2388,7 @@
         <v>16</v>
       </c>
       <c r="K16" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L16" s="16" t="s">
         <v>21</v>
@@ -2408,13 +2408,13 @@
         <v>21</v>
       </c>
       <c r="S16" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T16" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U16" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V16" s="12" t="s">
         <v>16</v>
@@ -2426,13 +2426,13 @@
         <v>90</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E17" s="8" t="s">
         <v>34</v>
@@ -2451,7 +2451,7 @@
         <v>16</v>
       </c>
       <c r="K17" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L17" s="16" t="s">
         <v>21</v>
@@ -2471,13 +2471,13 @@
         <v>21</v>
       </c>
       <c r="S17" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T17" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U17" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V17" s="12" t="s">
         <v>16</v>
@@ -2495,7 +2495,7 @@
         <v>16</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>34</v>
@@ -2536,13 +2536,13 @@
         <v>21</v>
       </c>
       <c r="S18" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T18" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U18" s="12" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="V18" s="12" t="s">
         <v>16</v>
@@ -2578,36 +2578,36 @@
         <v>21</v>
       </c>
       <c r="J19" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K19" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L19" s="16" t="s">
         <v>21</v>
       </c>
       <c r="M19" s="13"/>
       <c r="N19" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O19" s="6" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="P19" s="8"/>
       <c r="Q19" s="6" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="R19" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="S19" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="S19" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="T19" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U19" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V19" s="6" t="s">
         <v>21</v>
@@ -2643,7 +2643,7 @@
       </c>
       <c r="I20" s="8"/>
       <c r="J20" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K20" s="14" t="s">
         <v>21</v>
@@ -2663,16 +2663,16 @@
         <v>20</v>
       </c>
       <c r="R20" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S20" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T20" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U20" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V20" s="12" t="s">
         <v>16</v>
@@ -2690,7 +2690,7 @@
         <v>34</v>
       </c>
       <c r="D21" s="6" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>16</v>
@@ -2702,11 +2702,11 @@
         <v>21</v>
       </c>
       <c r="H21" s="6" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="I21" s="8"/>
       <c r="J21" s="6" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="K21" s="14" t="s">
         <v>21</v>
@@ -2724,10 +2724,10 @@
         <v>20</v>
       </c>
       <c r="R21" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S21" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T21" s="12" t="s">
         <v>16</v>
@@ -2767,16 +2767,16 @@
       </c>
       <c r="I22" s="8"/>
       <c r="J22" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K22" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L22" s="16" t="s">
         <v>21</v>
       </c>
       <c r="M22" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>16</v>
@@ -2789,10 +2789,10 @@
         <v>111</v>
       </c>
       <c r="R22" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S22" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T22" s="12" t="s">
         <v>16</v>
@@ -2856,16 +2856,16 @@
         <v>118</v>
       </c>
       <c r="R23" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S23" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T23" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U23" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V23" s="12" t="s">
         <v>16</v>
@@ -2899,7 +2899,7 @@
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K24" s="14" t="s">
         <v>21</v>
@@ -2919,10 +2919,10 @@
         <v>20</v>
       </c>
       <c r="R24" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S24" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T24" s="12" t="s">
         <v>16</v>
@@ -2964,17 +2964,17 @@
         <v>21</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K25" s="14" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="L25" s="16" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="M25" s="13"/>
       <c r="N25" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O25" s="6" t="s">
         <v>127</v>
@@ -2986,10 +2986,10 @@
         <v>128</v>
       </c>
       <c r="R25" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="S25" s="6" t="s">
         <v>243</v>
-      </c>
-      <c r="S25" s="6" t="s">
-        <v>244</v>
       </c>
       <c r="T25" s="12" t="s">
         <v>16</v>
@@ -3004,7 +3004,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="94.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
         <v>131</v>
       </c>
@@ -3012,59 +3012,59 @@
         <v>131</v>
       </c>
       <c r="C26" s="8" t="s">
-        <v>16</v>
+        <v>21</v>
       </c>
       <c r="D26" s="6" t="s">
+        <v>289</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F26" s="6" t="s">
         <v>132</v>
       </c>
-      <c r="E26" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F26" s="6" t="s">
+      <c r="G26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H26" s="6" t="s">
         <v>133</v>
       </c>
-      <c r="G26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H26" s="6" t="s">
-        <v>134</v>
-      </c>
       <c r="I26" s="8" t="s">
         <v>21</v>
       </c>
       <c r="J26" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K26" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L26" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M26" s="13"/>
       <c r="N26" s="6" t="s">
         <v>16</v>
       </c>
       <c r="O26" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="P26" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q26" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="P26" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q26" s="6" t="s">
-        <v>136</v>
-      </c>
       <c r="R26" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S26" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T26" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U26" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V26" s="12" t="s">
         <v>16</v>
@@ -3073,22 +3073,22 @@
     </row>
     <row r="27" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>258</v>
+      </c>
+      <c r="C27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>137</v>
       </c>
-      <c r="B27" s="7" t="s">
-        <v>259</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D27" s="6" t="s">
+      <c r="E27" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F27" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="G27" s="8" t="s">
         <v>21</v>
@@ -3101,7 +3101,7 @@
         <v>16</v>
       </c>
       <c r="K27" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L27" s="16" t="s">
         <v>21</v>
@@ -3111,23 +3111,23 @@
         <v>16</v>
       </c>
       <c r="O27" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P27" s="8"/>
       <c r="Q27" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R27" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S27" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T27" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U27" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V27" s="12" t="s">
         <v>16</v>
@@ -3136,22 +3136,22 @@
     </row>
     <row r="28" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C28" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D28" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>138</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F28" s="6" t="s">
-        <v>139</v>
       </c>
       <c r="G28" s="8" t="s">
         <v>21</v>
@@ -3164,7 +3164,7 @@
         <v>16</v>
       </c>
       <c r="K28" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L28" s="16" t="s">
         <v>21</v>
@@ -3174,23 +3174,23 @@
         <v>16</v>
       </c>
       <c r="O28" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="P28" s="8"/>
       <c r="Q28" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R28" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S28" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T28" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U28" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V28" s="12" t="s">
         <v>16</v>
@@ -3199,22 +3199,22 @@
     </row>
     <row r="29" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>142</v>
+      </c>
+      <c r="C29" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D29" s="6" t="s">
         <v>143</v>
       </c>
-      <c r="B29" s="7" t="s">
-        <v>143</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D29" s="6" t="s">
+      <c r="E29" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F29" s="6" t="s">
         <v>144</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>145</v>
       </c>
       <c r="G29" s="8" t="s">
         <v>21</v>
@@ -3229,17 +3229,17 @@
         <v>16</v>
       </c>
       <c r="K29" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L29" s="16" t="s">
         <v>21</v>
       </c>
       <c r="M29" s="13"/>
       <c r="N29" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O29" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="P29" s="8"/>
       <c r="Q29" s="6" t="s">
@@ -3249,13 +3249,13 @@
         <v>21</v>
       </c>
       <c r="S29" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T29" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U29" s="12" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="V29" s="12" t="s">
         <v>16</v>
@@ -3264,22 +3264,22 @@
     </row>
     <row r="30" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B30" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B30" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D30" s="6" t="s">
+      <c r="E30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F30" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E30" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F30" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G30" s="8" t="s">
         <v>21</v>
@@ -3297,10 +3297,10 @@
         <v>21</v>
       </c>
       <c r="L30" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M30" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N30" s="6" t="s">
         <v>16</v>
@@ -3312,45 +3312,45 @@
         <v>21</v>
       </c>
       <c r="Q30" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R30" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T30" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U30" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R30" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S30" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T30" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U30" s="12" t="s">
+      <c r="V30" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W30" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V30" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W30" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="31" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C31" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D31" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E31" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F31" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E31" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G31" s="8" t="s">
         <v>21</v>
@@ -3368,10 +3368,10 @@
         <v>21</v>
       </c>
       <c r="L31" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M31" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N31" s="6" t="s">
         <v>16</v>
@@ -3383,45 +3383,45 @@
         <v>21</v>
       </c>
       <c r="Q31" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R31" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T31" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U31" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R31" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S31" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T31" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U31" s="12" t="s">
+      <c r="V31" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W31" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V31" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W31" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="32" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C32" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D32" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E32" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F32" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E32" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G32" s="8" t="s">
         <v>21</v>
@@ -3439,10 +3439,10 @@
         <v>21</v>
       </c>
       <c r="L32" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M32" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N32" s="6" t="s">
         <v>16</v>
@@ -3454,45 +3454,45 @@
         <v>21</v>
       </c>
       <c r="Q32" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R32" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S32" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T32" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U32" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R32" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S32" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T32" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U32" s="12" t="s">
+      <c r="V32" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W32" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V32" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W32" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="33" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
+        <v>147</v>
+      </c>
+      <c r="B33" s="7" t="s">
+        <v>259</v>
+      </c>
+      <c r="C33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D33" s="6" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="7" t="s">
-        <v>260</v>
-      </c>
-      <c r="C33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D33" s="6" t="s">
+      <c r="E33" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F33" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E33" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G33" s="8" t="s">
         <v>21</v>
@@ -3510,10 +3510,10 @@
         <v>21</v>
       </c>
       <c r="L33" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M33" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N33" s="6" t="s">
         <v>16</v>
@@ -3525,45 +3525,45 @@
         <v>21</v>
       </c>
       <c r="Q33" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R33" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S33" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T33" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U33" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R33" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S33" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T33" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U33" s="12" t="s">
+      <c r="V33" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W33" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V33" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W33" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="34" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C34" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D34" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E34" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F34" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E34" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G34" s="8" t="s">
         <v>21</v>
@@ -3581,10 +3581,10 @@
         <v>21</v>
       </c>
       <c r="L34" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M34" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N34" s="6" t="s">
         <v>16</v>
@@ -3596,45 +3596,45 @@
         <v>21</v>
       </c>
       <c r="Q34" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R34" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S34" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T34" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U34" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R34" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S34" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T34" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U34" s="12" t="s">
+      <c r="V34" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W34" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V34" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W34" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="35" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C35" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D35" s="6" t="s">
+        <v>148</v>
+      </c>
+      <c r="E35" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F35" s="6" t="s">
         <v>149</v>
-      </c>
-      <c r="E35" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>150</v>
       </c>
       <c r="G35" s="8" t="s">
         <v>21</v>
@@ -3652,10 +3652,10 @@
         <v>21</v>
       </c>
       <c r="L35" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M35" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="N35" s="6" t="s">
         <v>16</v>
@@ -3667,51 +3667,51 @@
         <v>21</v>
       </c>
       <c r="Q35" s="6" t="s">
+        <v>150</v>
+      </c>
+      <c r="R35" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S35" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T35" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U35" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="R35" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S35" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T35" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U35" s="12" t="s">
+      <c r="V35" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W35" s="18" t="s">
         <v>152</v>
-      </c>
-      <c r="V35" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W35" s="18" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="36" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="B36" s="7" t="s">
+        <v>155</v>
+      </c>
+      <c r="C36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="6" t="s">
         <v>156</v>
       </c>
-      <c r="B36" s="7" t="s">
-        <v>156</v>
-      </c>
-      <c r="C36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D36" s="6" t="s">
+      <c r="E36" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F36" s="6" t="s">
         <v>157</v>
-      </c>
-      <c r="E36" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>158</v>
       </c>
       <c r="G36" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H36" s="6" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="I36" s="8" t="s">
         <v>16</v>
@@ -3734,19 +3734,19 @@
       </c>
       <c r="P36" s="8"/>
       <c r="Q36" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R36" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S36" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T36" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U36" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V36" s="12" t="s">
         <v>16</v>
@@ -3755,22 +3755,22 @@
     </row>
     <row r="37" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C37" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D37" s="6" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>16</v>
       </c>
       <c r="F37" s="6" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G37" s="8" t="s">
         <v>21</v>
@@ -3799,51 +3799,51 @@
       </c>
       <c r="P37" s="8"/>
       <c r="Q37" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R37" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S37" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T37" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U37" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V37" s="12" t="s">
         <v>21</v>
       </c>
       <c r="W37" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="38" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C38" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D38" s="6" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F38" s="6" t="s">
         <v>164</v>
       </c>
-      <c r="E38" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>165</v>
-      </c>
       <c r="G38" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H38" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I38" s="8" t="s">
         <v>16</v>
@@ -3866,55 +3866,55 @@
       </c>
       <c r="P38" s="8"/>
       <c r="Q38" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R38" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S38" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T38" s="12" t="s">
         <v>16</v>
       </c>
       <c r="U38" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="V38" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W38" s="12" t="s">
         <v>166</v>
-      </c>
-      <c r="V38" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W38" s="12" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="39" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="B39" s="7" t="s">
+        <v>167</v>
+      </c>
+      <c r="C39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D39" s="6" t="s">
         <v>168</v>
       </c>
-      <c r="B39" s="7" t="s">
-        <v>168</v>
-      </c>
-      <c r="C39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D39" s="6" t="s">
+      <c r="E39" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F39" s="6" t="s">
         <v>169</v>
-      </c>
-      <c r="E39" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>170</v>
       </c>
       <c r="G39" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H39" s="7" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="I39" s="8"/>
       <c r="J39" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K39" s="14" t="s">
         <v>21</v>
@@ -3931,19 +3931,19 @@
       </c>
       <c r="P39" s="8"/>
       <c r="Q39" s="6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="R39" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S39" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T39" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U39" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V39" s="12" t="s">
         <v>16</v>
@@ -3952,22 +3952,22 @@
     </row>
     <row r="40" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C40" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D40" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="E40" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F40" s="6" t="s">
         <v>173</v>
-      </c>
-      <c r="E40" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>174</v>
       </c>
       <c r="G40" s="8" t="s">
         <v>21</v>
@@ -3992,49 +3992,49 @@
         <v>16</v>
       </c>
       <c r="O40" s="6" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="P40" s="8"/>
       <c r="Q40" s="6" t="s">
+        <v>175</v>
+      </c>
+      <c r="R40" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="U40" s="12" t="s">
+        <v>263</v>
+      </c>
+      <c r="V40" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W40" s="18" t="s">
         <v>176</v>
-      </c>
-      <c r="R40" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S40" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T40" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="U40" s="12" t="s">
-        <v>264</v>
-      </c>
-      <c r="V40" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W40" s="18" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="41" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="B41" s="7" t="s">
+        <v>177</v>
+      </c>
+      <c r="C41" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D41" s="6" t="s">
         <v>178</v>
       </c>
-      <c r="B41" s="7" t="s">
-        <v>178</v>
-      </c>
-      <c r="C41" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D41" s="6" t="s">
+      <c r="E41" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F41" s="6" t="s">
         <v>179</v>
-      </c>
-      <c r="E41" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F41" s="6" t="s">
-        <v>180</v>
       </c>
       <c r="G41" s="8" t="s">
         <v>21</v>
@@ -4049,7 +4049,7 @@
         <v>16</v>
       </c>
       <c r="K41" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L41" s="16" t="s">
         <v>21</v>
@@ -4059,23 +4059,23 @@
         <v>16</v>
       </c>
       <c r="O41" s="6" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="P41" s="8"/>
       <c r="Q41" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="R41" s="6" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="S41" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T41" s="12" t="s">
         <v>16</v>
       </c>
       <c r="U41" s="12" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="V41" s="12" t="s">
         <v>16</v>
@@ -4084,28 +4084,28 @@
     </row>
     <row r="42" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C42" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D42" s="6" t="s">
+        <v>183</v>
+      </c>
+      <c r="E42" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F42" s="6" t="s">
         <v>184</v>
       </c>
-      <c r="E42" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>185</v>
-      </c>
       <c r="G42" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H42" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I42" s="8" t="s">
         <v>16</v>
@@ -4128,19 +4128,19 @@
       </c>
       <c r="P42" s="8"/>
       <c r="Q42" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="R42" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S42" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T42" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="U42" s="12" t="s">
         <v>186</v>
-      </c>
-      <c r="R42" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S42" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T42" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="U42" s="12" t="s">
-        <v>187</v>
       </c>
       <c r="V42" s="12" t="s">
         <v>16</v>
@@ -4149,22 +4149,22 @@
     </row>
     <row r="43" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
+        <v>187</v>
+      </c>
+      <c r="B43" s="7" t="s">
+        <v>260</v>
+      </c>
+      <c r="C43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D43" s="6" t="s">
         <v>188</v>
       </c>
-      <c r="B43" s="7" t="s">
-        <v>261</v>
-      </c>
-      <c r="C43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D43" s="6" t="s">
+      <c r="E43" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F43" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="E43" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G43" s="8" t="s">
         <v>21</v>
@@ -4174,7 +4174,7 @@
       </c>
       <c r="I43" s="8"/>
       <c r="J43" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K43" s="14" t="s">
         <v>21</v>
@@ -4187,23 +4187,23 @@
         <v>16</v>
       </c>
       <c r="O43" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P43" s="8"/>
       <c r="Q43" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R43" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S43" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T43" s="12" t="s">
         <v>16</v>
       </c>
       <c r="U43" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V43" s="12" t="s">
         <v>16</v>
@@ -4212,22 +4212,22 @@
     </row>
     <row r="44" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D44" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E44" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>189</v>
-      </c>
-      <c r="E44" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>190</v>
       </c>
       <c r="G44" s="8" t="s">
         <v>21</v>
@@ -4237,7 +4237,7 @@
       </c>
       <c r="I44" s="8"/>
       <c r="J44" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K44" s="14" t="s">
         <v>21</v>
@@ -4250,23 +4250,23 @@
         <v>16</v>
       </c>
       <c r="O44" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P44" s="8"/>
       <c r="Q44" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R44" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S44" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T44" s="12" t="s">
         <v>16</v>
       </c>
       <c r="U44" s="12" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="V44" s="12" t="s">
         <v>16</v>
@@ -4275,22 +4275,22 @@
     </row>
     <row r="45" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="B45" s="7" t="s">
+        <v>193</v>
+      </c>
+      <c r="C45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D45" s="6" t="s">
         <v>194</v>
       </c>
-      <c r="B45" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D45" s="6" t="s">
+      <c r="E45" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F45" s="6" t="s">
         <v>195</v>
-      </c>
-      <c r="E45" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>196</v>
       </c>
       <c r="G45" s="8" t="s">
         <v>21</v>
@@ -4308,34 +4308,34 @@
         <v>21</v>
       </c>
       <c r="L45" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="M45" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="N45" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O45" s="6" t="s">
+        <v>196</v>
+      </c>
+      <c r="P45" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q45" s="6" t="s">
         <v>197</v>
       </c>
-      <c r="P45" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q45" s="6" t="s">
+      <c r="R45" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S45" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="T45" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U45" s="12" t="s">
         <v>198</v>
-      </c>
-      <c r="R45" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S45" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="T45" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U45" s="12" t="s">
-        <v>199</v>
       </c>
       <c r="V45" s="12" t="s">
         <v>16</v>
@@ -4344,32 +4344,32 @@
     </row>
     <row r="46" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="B46" s="7" t="s">
+        <v>199</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D46" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="B46" s="7" t="s">
-        <v>200</v>
-      </c>
-      <c r="C46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D46" s="6" t="s">
+      <c r="E46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F46" s="6" t="s">
         <v>201</v>
-      </c>
-      <c r="E46" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F46" s="6" t="s">
-        <v>202</v>
       </c>
       <c r="G46" s="8" t="s">
         <v>34</v>
       </c>
       <c r="H46" s="6" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="I46" s="8"/>
       <c r="J46" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K46" s="14" t="s">
         <v>21</v>
@@ -4382,23 +4382,23 @@
         <v>16</v>
       </c>
       <c r="O46" s="6" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P46" s="8"/>
       <c r="Q46" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R46" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S46" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T46" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U46" s="12" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="V46" s="12" t="s">
         <v>16</v>
@@ -4407,100 +4407,100 @@
     </row>
     <row r="47" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="B47" s="7" t="s">
+        <v>203</v>
+      </c>
+      <c r="C47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>194</v>
+      </c>
+      <c r="E47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F47" s="6" t="s">
         <v>204</v>
       </c>
-      <c r="B47" s="7" t="s">
-        <v>204</v>
-      </c>
-      <c r="C47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D47" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="E47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F47" s="6" t="s">
+      <c r="G47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="I47" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K47" s="14" t="s">
+        <v>238</v>
+      </c>
+      <c r="L47" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="M47" s="13" t="s">
+        <v>248</v>
+      </c>
+      <c r="N47" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="O47" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="G47" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H47" s="6" t="s">
-        <v>275</v>
-      </c>
-      <c r="I47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="J47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K47" s="14" t="s">
-        <v>239</v>
-      </c>
-      <c r="L47" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="M47" s="13" t="s">
-        <v>249</v>
-      </c>
-      <c r="N47" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="O47" s="6" t="s">
+      <c r="P47" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q47" s="6" t="s">
         <v>206</v>
       </c>
-      <c r="P47" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q47" s="6" t="s">
-        <v>207</v>
-      </c>
       <c r="R47" s="6" t="s">
         <v>21</v>
       </c>
       <c r="S47" s="6" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="T47" s="12" t="s">
         <v>34</v>
       </c>
       <c r="U47" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="V47" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="W47" s="12" t="s">
         <v>208</v>
-      </c>
-      <c r="V47" s="12" t="s">
-        <v>21</v>
-      </c>
-      <c r="W47" s="12" t="s">
-        <v>209</v>
       </c>
     </row>
     <row r="48" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
+        <v>209</v>
+      </c>
+      <c r="B48" s="7" t="s">
+        <v>261</v>
+      </c>
+      <c r="C48" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D48" s="6" t="s">
         <v>210</v>
       </c>
-      <c r="B48" s="7" t="s">
-        <v>262</v>
-      </c>
-      <c r="C48" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D48" s="6" t="s">
+      <c r="E48" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F48" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E48" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F48" s="6" t="s">
+      <c r="G48" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H48" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G48" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H48" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="I48" s="8" t="s">
         <v>21</v>
       </c>
@@ -4508,17 +4508,17 @@
         <v>16</v>
       </c>
       <c r="K48" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L48" s="16" t="s">
         <v>34</v>
       </c>
       <c r="M48" s="13"/>
       <c r="N48" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O48" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P48" s="8"/>
       <c r="Q48" s="6" t="s">
@@ -4528,13 +4528,13 @@
         <v>21</v>
       </c>
       <c r="S48" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T48" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U48" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V48" s="12" t="s">
         <v>16</v>
@@ -4543,29 +4543,29 @@
     </row>
     <row r="49" spans="1:23" ht="63" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="C49" s="8" t="s">
         <v>16</v>
       </c>
       <c r="D49" s="6" t="s">
+        <v>210</v>
+      </c>
+      <c r="E49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F49" s="6" t="s">
         <v>211</v>
       </c>
-      <c r="E49" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F49" s="6" t="s">
+      <c r="G49" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H49" s="6" t="s">
         <v>212</v>
       </c>
-      <c r="G49" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="H49" s="6" t="s">
-        <v>213</v>
-      </c>
       <c r="I49" s="8" t="s">
         <v>21</v>
       </c>
@@ -4573,17 +4573,17 @@
         <v>16</v>
       </c>
       <c r="K49" s="14" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="L49" s="16" t="s">
         <v>34</v>
       </c>
       <c r="M49" s="13"/>
       <c r="N49" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O49" s="6" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="P49" s="8"/>
       <c r="Q49" s="6" t="s">
@@ -4593,13 +4593,13 @@
         <v>21</v>
       </c>
       <c r="S49" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="T49" s="12" t="s">
         <v>21</v>
       </c>
       <c r="U49" s="12" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="V49" s="12" t="s">
         <v>16</v>
@@ -4608,22 +4608,22 @@
     </row>
     <row r="50" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="C50" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D50" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="E50" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F50" s="6" t="s">
         <v>217</v>
-      </c>
-      <c r="E50" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>218</v>
       </c>
       <c r="G50" s="8" t="s">
         <v>21</v>
@@ -4643,7 +4643,7 @@
       </c>
       <c r="M50" s="13"/>
       <c r="N50" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O50" s="6" t="s">
         <v>80</v>
@@ -4651,16 +4651,16 @@
       <c r="P50" s="8"/>
       <c r="Q50" s="6"/>
       <c r="R50" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="S50" s="6" t="s">
         <v>243</v>
       </c>
-      <c r="S50" s="6" t="s">
-        <v>244</v>
-      </c>
       <c r="T50" s="12" t="s">
         <v>16</v>
       </c>
       <c r="U50" s="12" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="V50" s="12" t="s">
         <v>16</v>
@@ -4669,28 +4669,28 @@
     </row>
     <row r="51" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="B51" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D51" s="6" t="s">
         <v>220</v>
       </c>
-      <c r="B51" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D51" s="6" t="s">
+      <c r="E51" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F51" s="6" t="s">
         <v>221</v>
       </c>
-      <c r="E51" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>222</v>
-      </c>
       <c r="G51" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H51" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I51" s="8" t="s">
         <v>21</v>
@@ -4706,28 +4706,28 @@
       </c>
       <c r="M51" s="13"/>
       <c r="N51" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="O51" s="6" t="s">
+        <v>222</v>
+      </c>
+      <c r="P51" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q51" s="6" t="s">
         <v>223</v>
       </c>
-      <c r="P51" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q51" s="6" t="s">
+      <c r="R51" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S51" s="6" t="s">
+        <v>243</v>
+      </c>
+      <c r="T51" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U51" s="12" t="s">
         <v>224</v>
-      </c>
-      <c r="R51" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="S51" s="6" t="s">
-        <v>244</v>
-      </c>
-      <c r="T51" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U51" s="12" t="s">
-        <v>225</v>
       </c>
       <c r="V51" s="12" t="s">
         <v>16</v>
@@ -4736,22 +4736,22 @@
     </row>
     <row r="52" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B52" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="C52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D52" s="6" t="s">
+        <v>220</v>
+      </c>
+      <c r="E52" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="F52" s="6" t="s">
         <v>226</v>
-      </c>
-      <c r="B52" s="7" t="s">
-        <v>226</v>
-      </c>
-      <c r="C52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D52" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="E52" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>227</v>
       </c>
       <c r="G52" s="8" t="s">
         <v>16</v>
@@ -4759,10 +4759,10 @@
       <c r="H52" s="6"/>
       <c r="I52" s="8"/>
       <c r="J52" s="6" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="K52" s="14" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="L52" s="13" t="s">
         <v>21</v>
@@ -4776,51 +4776,51 @@
       </c>
       <c r="P52" s="8"/>
       <c r="Q52" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="R52" s="6" t="s">
+        <v>242</v>
+      </c>
+      <c r="S52" s="6" t="s">
+        <v>284</v>
+      </c>
+      <c r="T52" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="U52" s="12" t="s">
         <v>228</v>
-      </c>
-      <c r="R52" s="6" t="s">
-        <v>243</v>
-      </c>
-      <c r="S52" s="6" t="s">
-        <v>285</v>
-      </c>
-      <c r="T52" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="U52" s="12" t="s">
-        <v>229</v>
       </c>
       <c r="V52" s="12" t="s">
         <v>34</v>
       </c>
       <c r="W52" s="12" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="53" spans="1:23" ht="60" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C53" s="8" t="s">
         <v>34</v>
       </c>
       <c r="D53" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="E53" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F53" s="6" t="s">
         <v>232</v>
       </c>
-      <c r="E53" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>233</v>
-      </c>
       <c r="G53" s="8" t="s">
         <v>21</v>
       </c>
       <c r="H53" s="6" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I53" s="8"/>
       <c r="J53" s="6" t="s">
@@ -4833,7 +4833,7 @@
         <v>21</v>
       </c>
       <c r="M53" s="16" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="N53" s="6" t="s">
         <v>16</v>
@@ -4843,19 +4843,19 @@
       </c>
       <c r="P53" s="8"/>
       <c r="Q53" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="R53" s="6" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="S53" s="6" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T53" s="12" t="s">
         <v>34</v>
       </c>
       <c r="U53" s="12" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="V53" s="12" t="s">
         <v>16</v>
@@ -4864,28 +4864,28 @@
     </row>
     <row r="54" spans="1:23" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A54" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>279</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D54" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="E54" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="F54" s="20" t="s">
         <v>280</v>
       </c>
-      <c r="B54" s="5" t="s">
-        <v>280</v>
-      </c>
-      <c r="C54" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="D54" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="E54" s="19" t="s">
-        <v>16</v>
-      </c>
-      <c r="F54" s="20" t="s">
-        <v>281</v>
-      </c>
       <c r="G54" s="19" t="s">
         <v>21</v>
       </c>
       <c r="H54" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="I54" s="19"/>
       <c r="J54" s="6" t="s">
@@ -4898,7 +4898,7 @@
         <v>21</v>
       </c>
       <c r="M54" s="11" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="N54" s="6" t="s">
         <v>16</v>
@@ -4906,19 +4906,19 @@
       <c r="O54" s="19"/>
       <c r="P54" s="19"/>
       <c r="Q54" s="19" t="s">
+        <v>282</v>
+      </c>
+      <c r="R54" s="6" t="s">
+        <v>245</v>
+      </c>
+      <c r="S54" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="T54" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="U54" s="20" t="s">
         <v>283</v>
-      </c>
-      <c r="R54" s="6" t="s">
-        <v>246</v>
-      </c>
-      <c r="S54" s="19" t="s">
-        <v>285</v>
-      </c>
-      <c r="T54" s="20" t="s">
-        <v>16</v>
-      </c>
-      <c r="U54" s="20" t="s">
-        <v>284</v>
       </c>
       <c r="V54" s="21" t="s">
         <v>16</v>
@@ -4927,55 +4927,55 @@
     </row>
     <row r="55" spans="1:23" ht="47.25" x14ac:dyDescent="0.4">
       <c r="A55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D55" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="B55" s="1" t="s">
-        <v>287</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D55" s="1" t="s">
+      <c r="E55" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>280</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="H55" s="2" t="s">
+        <v>272</v>
+      </c>
+      <c r="J55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="K55" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="L55" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="N55" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="Q55" s="1" t="s">
         <v>288</v>
       </c>
-      <c r="E55" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="F55" s="20" t="s">
-        <v>281</v>
-      </c>
-      <c r="G55" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>273</v>
-      </c>
-      <c r="J55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="K55" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="L55" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="N55" s="6" t="s">
-        <v>16</v>
-      </c>
-      <c r="Q55" s="1" t="s">
-        <v>289</v>
-      </c>
       <c r="R55" s="6" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="S55" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="T55" s="2" t="s">
         <v>16</v>
       </c>
       <c r="U55" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="V55" s="3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
Updating of rmarkdown to fit publication requirements (eg tables to the back) Corrections as recommended post-thesis submission
Corrected quality evaluation error in quality_scores
</commit_message>
<xml_diff>
--- a/quality_review.xlsx
+++ b/quality_review.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gla-my.sharepoint.com/personal/2509920f_student_gla_ac_uk/Documents/DClin/Deliverables/Systematic Review/Writeup/DCLIN_SR_git/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="634" documentId="8_{BDA90F51-975A-4A3A-9E3C-A0EF38026AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FF755F46-328C-4F3E-9BED-656612325F0D}"/>
+  <xr:revisionPtr revIDLastSave="635" documentId="8_{BDA90F51-975A-4A3A-9E3C-A0EF38026AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B0E4B5D5-E76B-4410-AA7B-E50C6C100C28}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{960BDED2-1FF1-4B58-9DE1-81C8DE898166}"/>
+    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11500" xr2:uid="{960BDED2-1FF1-4B58-9DE1-81C8DE898166}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1448,41 +1448,41 @@
   <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="I60" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="M9" sqref="M9"/>
+      <selection pane="bottomRight" activeCell="N64" sqref="N64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="26.25" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="26" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="137.140625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.85546875" style="14" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="49.85546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.5703125" style="19" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.7109375" style="15" customWidth="1"/>
-    <col min="12" max="12" width="13.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="49.140625" style="3" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="24.140625" style="19" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="8.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="76.42578125" style="19" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="137.1796875" style="13" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.81640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="49.81640625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.54296875" style="19" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.7265625" style="15" customWidth="1"/>
+    <col min="12" max="12" width="13.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="49.1796875" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.1796875" style="19" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.453125" style="13" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="76.453125" style="19" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="23" style="3" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" style="13" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.5703125" style="14" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="95.7109375" style="14" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" style="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="82.140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="3"/>
+    <col min="19" max="19" width="19.54296875" style="13" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="13.54296875" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="95.7265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.54296875" style="17" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="82.1796875" style="14" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>246</v>
       </c>
@@ -1553,7 +1553,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" ht="31" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>15</v>
       </c>
@@ -1618,7 +1618,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="3" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A3" s="8" t="s">
         <v>24</v>
       </c>
@@ -1681,7 +1681,7 @@
       </c>
       <c r="W3" s="2"/>
     </row>
-    <row r="4" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" ht="31" x14ac:dyDescent="0.35">
       <c r="A4" s="8" t="s">
         <v>28</v>
       </c>
@@ -1744,7 +1744,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A5" s="8" t="s">
         <v>32</v>
       </c>
@@ -1809,7 +1809,7 @@
       </c>
       <c r="W5" s="2"/>
     </row>
-    <row r="6" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A6" s="8" t="s">
         <v>38</v>
       </c>
@@ -1876,7 +1876,7 @@
       </c>
       <c r="W6" s="2"/>
     </row>
-    <row r="7" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A7" s="8" t="s">
         <v>42</v>
       </c>
@@ -1939,7 +1939,7 @@
       </c>
       <c r="W7" s="2"/>
     </row>
-    <row r="8" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A8" s="8" t="s">
         <v>47</v>
       </c>
@@ -2004,7 +2004,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="9" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A9" s="8" t="s">
         <v>53</v>
       </c>
@@ -2069,7 +2069,7 @@
       </c>
       <c r="W9" s="2"/>
     </row>
-    <row r="10" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A10" s="8" t="s">
         <v>311</v>
       </c>
@@ -2134,7 +2134,7 @@
       </c>
       <c r="W10" s="2"/>
     </row>
-    <row r="11" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A11" s="8" t="s">
         <v>312</v>
       </c>
@@ -2199,7 +2199,7 @@
       </c>
       <c r="W11" s="2"/>
     </row>
-    <row r="12" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A12" s="8" t="s">
         <v>62</v>
       </c>
@@ -2262,7 +2262,7 @@
       </c>
       <c r="W12" s="2"/>
     </row>
-    <row r="13" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A13" s="8" t="s">
         <v>65</v>
       </c>
@@ -2327,7 +2327,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="14" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A14" s="8" t="s">
         <v>69</v>
       </c>
@@ -2392,7 +2392,7 @@
       </c>
       <c r="W14" s="2"/>
     </row>
-    <row r="15" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A15" s="8" t="s">
         <v>73</v>
       </c>
@@ -2455,7 +2455,7 @@
       </c>
       <c r="W15" s="2"/>
     </row>
-    <row r="16" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A16" s="8" t="s">
         <v>78</v>
       </c>
@@ -2522,7 +2522,7 @@
       </c>
       <c r="W16" s="2"/>
     </row>
-    <row r="17" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A17" s="8" t="s">
         <v>82</v>
       </c>
@@ -2585,7 +2585,7 @@
       </c>
       <c r="W17" s="2"/>
     </row>
-    <row r="18" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A18" s="8" t="s">
         <v>85</v>
       </c>
@@ -2648,7 +2648,7 @@
       </c>
       <c r="W18" s="2"/>
     </row>
-    <row r="19" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A19" s="8" t="s">
         <v>86</v>
       </c>
@@ -2713,7 +2713,7 @@
       </c>
       <c r="W19" s="2"/>
     </row>
-    <row r="20" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A20" s="8" t="s">
         <v>89</v>
       </c>
@@ -2780,7 +2780,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:23" ht="31" x14ac:dyDescent="0.35">
       <c r="A21" s="8" t="s">
         <v>94</v>
       </c>
@@ -2843,7 +2843,7 @@
       </c>
       <c r="W21" s="2"/>
     </row>
-    <row r="22" spans="1:23" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:23" ht="31" x14ac:dyDescent="0.35">
       <c r="A22" s="8" t="s">
         <v>99</v>
       </c>
@@ -2904,7 +2904,7 @@
       </c>
       <c r="W22" s="2"/>
     </row>
-    <row r="23" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A23" s="8" t="s">
         <v>103</v>
       </c>
@@ -2971,7 +2971,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="24" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A24" s="8" t="s">
         <v>109</v>
       </c>
@@ -3034,7 +3034,7 @@
       </c>
       <c r="W24" s="2"/>
     </row>
-    <row r="25" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A25" s="8" t="s">
         <v>114</v>
       </c>
@@ -3103,7 +3103,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="26" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A26" s="8" t="s">
         <v>121</v>
       </c>
@@ -3170,7 +3170,7 @@
       </c>
       <c r="W26" s="2"/>
     </row>
-    <row r="27" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A27" s="8" t="s">
         <v>126</v>
       </c>
@@ -3233,7 +3233,7 @@
       </c>
       <c r="W27" s="2"/>
     </row>
-    <row r="28" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A28" s="8" t="s">
         <v>131</v>
       </c>
@@ -3296,7 +3296,7 @@
       </c>
       <c r="W28" s="2"/>
     </row>
-    <row r="29" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A29" s="8" t="s">
         <v>132</v>
       </c>
@@ -3361,7 +3361,7 @@
       </c>
       <c r="W29" s="2"/>
     </row>
-    <row r="30" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A30" s="8" t="s">
         <v>137</v>
       </c>
@@ -3432,7 +3432,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="31" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A31" s="8" t="s">
         <v>143</v>
       </c>
@@ -3503,7 +3503,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A32" s="8" t="s">
         <v>144</v>
       </c>
@@ -3574,7 +3574,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="33" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A33" s="8" t="s">
         <v>280</v>
       </c>
@@ -3645,7 +3645,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="34" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A34" s="8" t="s">
         <v>281</v>
       </c>
@@ -3716,7 +3716,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="35" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A35" s="8" t="s">
         <v>282</v>
       </c>
@@ -3787,7 +3787,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="36" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A36" s="8" t="s">
         <v>145</v>
       </c>
@@ -3852,7 +3852,7 @@
       </c>
       <c r="W36" s="2"/>
     </row>
-    <row r="37" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A37" s="8" t="s">
         <v>150</v>
       </c>
@@ -3919,7 +3919,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="38" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A38" s="8" t="s">
         <v>152</v>
       </c>
@@ -3986,7 +3986,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="39" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A39" s="8" t="s">
         <v>157</v>
       </c>
@@ -4049,7 +4049,7 @@
       </c>
       <c r="W39" s="2"/>
     </row>
-    <row r="40" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A40" s="8" t="s">
         <v>161</v>
       </c>
@@ -4116,7 +4116,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:23" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A41" s="8" t="s">
         <v>167</v>
       </c>
@@ -4181,7 +4181,7 @@
       </c>
       <c r="W41" s="2"/>
     </row>
-    <row r="42" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A42" s="8" t="s">
         <v>172</v>
       </c>
@@ -4246,7 +4246,7 @@
       </c>
       <c r="W42" s="2"/>
     </row>
-    <row r="43" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A43" s="8" t="s">
         <v>177</v>
       </c>
@@ -4309,7 +4309,7 @@
       </c>
       <c r="W43" s="2"/>
     </row>
-    <row r="44" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A44" s="8" t="s">
         <v>182</v>
       </c>
@@ -4372,7 +4372,7 @@
       </c>
       <c r="W44" s="2"/>
     </row>
-    <row r="45" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A45" s="8" t="s">
         <v>183</v>
       </c>
@@ -4441,7 +4441,7 @@
       </c>
       <c r="W45" s="2"/>
     </row>
-    <row r="46" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A46" s="8" t="s">
         <v>189</v>
       </c>
@@ -4504,7 +4504,7 @@
       </c>
       <c r="W46" s="2"/>
     </row>
-    <row r="47" spans="1:23" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:23" ht="77.5" x14ac:dyDescent="0.35">
       <c r="A47" s="8" t="s">
         <v>193</v>
       </c>
@@ -4575,7 +4575,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="48" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A48" s="8" t="s">
         <v>199</v>
       </c>
@@ -4640,7 +4640,7 @@
       </c>
       <c r="W48" s="2"/>
     </row>
-    <row r="49" spans="1:23" ht="63" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:23" ht="62" x14ac:dyDescent="0.35">
       <c r="A49" s="8" t="s">
         <v>204</v>
       </c>
@@ -4705,7 +4705,7 @@
       </c>
       <c r="W49" s="2"/>
     </row>
-    <row r="50" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A50" s="8" t="s">
         <v>205</v>
       </c>
@@ -4766,7 +4766,7 @@
       </c>
       <c r="W50" s="2"/>
     </row>
-    <row r="51" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A51" s="8" t="s">
         <v>209</v>
       </c>
@@ -4833,7 +4833,7 @@
       </c>
       <c r="W51" s="2"/>
     </row>
-    <row r="52" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A52" s="8" t="s">
         <v>215</v>
       </c>
@@ -4896,7 +4896,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="53" spans="1:23" ht="47.25" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:23" ht="46.5" x14ac:dyDescent="0.35">
       <c r="A53" s="8" t="s">
         <v>220</v>
       </c>
@@ -4961,7 +4961,7 @@
       </c>
       <c r="W53" s="2"/>
     </row>
-    <row r="54" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>268</v>
       </c>
@@ -5024,7 +5024,7 @@
       </c>
       <c r="W54" s="12"/>
     </row>
-    <row r="55" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:23" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A55" s="13" t="s">
         <v>275</v>
       </c>
@@ -5080,7 +5080,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="56" spans="1:23" ht="110.25" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:23" ht="108.5" x14ac:dyDescent="0.35">
       <c r="A56" s="13" t="s">
         <v>307</v>
       </c>
@@ -5133,7 +5133,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A57" s="13" t="s">
         <v>284</v>
       </c>
@@ -5189,7 +5189,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="58" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A58" s="13" t="s">
         <v>308</v>
       </c>
@@ -5242,7 +5242,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="59" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A59" s="13" t="s">
         <v>309</v>
       </c>
@@ -5295,7 +5295,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="60" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A60" s="13" t="s">
         <v>296</v>
       </c>
@@ -5348,7 +5348,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="61" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A61" s="13" t="s">
         <v>297</v>
       </c>
@@ -5401,7 +5401,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="62" spans="1:23" ht="30" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A62" s="13" t="s">
         <v>298</v>
       </c>
@@ -5454,7 +5454,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="63" spans="1:23" ht="90" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:23" ht="87" x14ac:dyDescent="0.35">
       <c r="A63" s="13" t="s">
         <v>299</v>
       </c>
@@ -5510,7 +5510,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="64" spans="1:23" ht="45" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:23" ht="29" x14ac:dyDescent="0.35">
       <c r="A64" s="13" t="s">
         <v>305</v>
       </c>
@@ -5539,7 +5539,7 @@
         <v>16</v>
       </c>
       <c r="K64" s="15" t="s">
-        <v>34</v>
+        <v>21</v>
       </c>
       <c r="L64" s="13" t="s">
         <v>21</v>

</xml_diff>